<commit_message>
corrected inflation rates and added calculations, also highlighted spreadsheets: relevant cells in green; relevant columns in yellow; final inflation and special calibration of other in orange
</commit_message>
<xml_diff>
--- a/WPI-sectors-2022-2021.xlsx
+++ b/WPI-sectors-2022-2021.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uq-my.sharepoint.com/personal/uqpocall_uq_edu_au/Documents/inflation-one-pager-20220607/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrickocal_mchome/Documents/_uq-aibe/explainer-series/inflation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{5DC645EF-D374-3B42-9097-DFA6323A05E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{25EF64C5-9E94-EF49-957A-2BCFBD4E9959}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F6B1089-49BD-4347-98B2-BA531A5EC22A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="30080" windowHeight="33340" xr2:uid="{DF2A599F-A237-F346-845F-21B4E6A0095D}"/>
   </bookViews>
@@ -17,6 +17,110 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$1</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$A$10</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$B$19</definedName>
+    <definedName name="_xlchart.v1.100" hidden="1">Sheet1!$B$12</definedName>
+    <definedName name="_xlchart.v1.101" hidden="1">Sheet1!$B$19</definedName>
+    <definedName name="_xlchart.v1.102" hidden="1">Sheet1!$B$20</definedName>
+    <definedName name="_xlchart.v1.103" hidden="1">Sheet1!$B$7</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$B$20</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$B$7</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$A$1</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$A$10</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$A$12</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$A$19</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$A$20</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">Sheet1!$A$2:$B$2</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">Sheet1!$A$7</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$A$12</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">Sheet1!$B$10</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">Sheet1!$B$12</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">Sheet1!$B$19</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">Sheet1!$B$20</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">Sheet1!$B$7</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">Sheet1!$A$1</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">Sheet1!$A$10</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">Sheet1!$A$12</definedName>
+    <definedName name="_xlchart.v1.29" hidden="1">Sheet1!$A$19</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$A$19</definedName>
+    <definedName name="_xlchart.v1.30" hidden="1">Sheet1!$A$20</definedName>
+    <definedName name="_xlchart.v1.31" hidden="1">Sheet1!$A$2:$B$2</definedName>
+    <definedName name="_xlchart.v1.32" hidden="1">Sheet1!$A$7</definedName>
+    <definedName name="_xlchart.v1.33" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.34" hidden="1">Sheet1!$B$10</definedName>
+    <definedName name="_xlchart.v1.35" hidden="1">Sheet1!$B$12</definedName>
+    <definedName name="_xlchart.v1.36" hidden="1">Sheet1!$B$19</definedName>
+    <definedName name="_xlchart.v1.37" hidden="1">Sheet1!$B$20</definedName>
+    <definedName name="_xlchart.v1.38" hidden="1">Sheet1!$B$7</definedName>
+    <definedName name="_xlchart.v1.39" hidden="1">Sheet1!$A$1</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$A$20</definedName>
+    <definedName name="_xlchart.v1.40" hidden="1">Sheet1!$A$10</definedName>
+    <definedName name="_xlchart.v1.41" hidden="1">Sheet1!$A$12</definedName>
+    <definedName name="_xlchart.v1.42" hidden="1">Sheet1!$A$19</definedName>
+    <definedName name="_xlchart.v1.43" hidden="1">Sheet1!$A$20</definedName>
+    <definedName name="_xlchart.v1.44" hidden="1">Sheet1!$A$2:$B$2</definedName>
+    <definedName name="_xlchart.v1.45" hidden="1">Sheet1!$A$7</definedName>
+    <definedName name="_xlchart.v1.46" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.47" hidden="1">Sheet1!$B$10</definedName>
+    <definedName name="_xlchart.v1.48" hidden="1">Sheet1!$B$12</definedName>
+    <definedName name="_xlchart.v1.49" hidden="1">Sheet1!$B$19</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$A$2:$B$2</definedName>
+    <definedName name="_xlchart.v1.50" hidden="1">Sheet1!$B$20</definedName>
+    <definedName name="_xlchart.v1.51" hidden="1">Sheet1!$B$7</definedName>
+    <definedName name="_xlchart.v1.52" hidden="1">Sheet1!$A$1</definedName>
+    <definedName name="_xlchart.v1.53" hidden="1">Sheet1!$A$10</definedName>
+    <definedName name="_xlchart.v1.54" hidden="1">Sheet1!$A$12</definedName>
+    <definedName name="_xlchart.v1.55" hidden="1">Sheet1!$A$19</definedName>
+    <definedName name="_xlchart.v1.56" hidden="1">Sheet1!$A$20</definedName>
+    <definedName name="_xlchart.v1.57" hidden="1">Sheet1!$A$2:$B$2</definedName>
+    <definedName name="_xlchart.v1.58" hidden="1">Sheet1!$A$7</definedName>
+    <definedName name="_xlchart.v1.59" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$A$7</definedName>
+    <definedName name="_xlchart.v1.60" hidden="1">Sheet1!$B$10</definedName>
+    <definedName name="_xlchart.v1.61" hidden="1">Sheet1!$B$12</definedName>
+    <definedName name="_xlchart.v1.62" hidden="1">Sheet1!$B$19</definedName>
+    <definedName name="_xlchart.v1.63" hidden="1">Sheet1!$B$20</definedName>
+    <definedName name="_xlchart.v1.64" hidden="1">Sheet1!$B$7</definedName>
+    <definedName name="_xlchart.v1.65" hidden="1">Sheet1!$A$1</definedName>
+    <definedName name="_xlchart.v1.66" hidden="1">Sheet1!$A$10</definedName>
+    <definedName name="_xlchart.v1.67" hidden="1">Sheet1!$A$12</definedName>
+    <definedName name="_xlchart.v1.68" hidden="1">Sheet1!$A$19</definedName>
+    <definedName name="_xlchart.v1.69" hidden="1">Sheet1!$A$20</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.70" hidden="1">Sheet1!$A$2:$B$2</definedName>
+    <definedName name="_xlchart.v1.71" hidden="1">Sheet1!$A$7</definedName>
+    <definedName name="_xlchart.v1.72" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.73" hidden="1">Sheet1!$B$10</definedName>
+    <definedName name="_xlchart.v1.74" hidden="1">Sheet1!$B$12</definedName>
+    <definedName name="_xlchart.v1.75" hidden="1">Sheet1!$B$19</definedName>
+    <definedName name="_xlchart.v1.76" hidden="1">Sheet1!$B$20</definedName>
+    <definedName name="_xlchart.v1.77" hidden="1">Sheet1!$B$7</definedName>
+    <definedName name="_xlchart.v1.78" hidden="1">Sheet1!$A$1</definedName>
+    <definedName name="_xlchart.v1.79" hidden="1">Sheet1!$A$10</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$B$10</definedName>
+    <definedName name="_xlchart.v1.80" hidden="1">Sheet1!$A$12</definedName>
+    <definedName name="_xlchart.v1.81" hidden="1">Sheet1!$A$19</definedName>
+    <definedName name="_xlchart.v1.82" hidden="1">Sheet1!$A$20</definedName>
+    <definedName name="_xlchart.v1.83" hidden="1">Sheet1!$A$2:$B$2</definedName>
+    <definedName name="_xlchart.v1.84" hidden="1">Sheet1!$A$7</definedName>
+    <definedName name="_xlchart.v1.85" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.86" hidden="1">Sheet1!$B$10</definedName>
+    <definedName name="_xlchart.v1.87" hidden="1">Sheet1!$B$12</definedName>
+    <definedName name="_xlchart.v1.88" hidden="1">Sheet1!$B$19</definedName>
+    <definedName name="_xlchart.v1.89" hidden="1">Sheet1!$B$20</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$B$12</definedName>
+    <definedName name="_xlchart.v1.90" hidden="1">Sheet1!$B$7</definedName>
+    <definedName name="_xlchart.v1.91" hidden="1">Sheet1!$A$1</definedName>
+    <definedName name="_xlchart.v1.92" hidden="1">Sheet1!$A$10</definedName>
+    <definedName name="_xlchart.v1.93" hidden="1">Sheet1!$A$12</definedName>
+    <definedName name="_xlchart.v1.94" hidden="1">Sheet1!$A$19</definedName>
+    <definedName name="_xlchart.v1.95" hidden="1">Sheet1!$A$20</definedName>
+    <definedName name="_xlchart.v1.96" hidden="1">Sheet1!$A$2:$B$2</definedName>
+    <definedName name="_xlchart.v1.97" hidden="1">Sheet1!$A$7</definedName>
+    <definedName name="_xlchart.v1.98" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.99" hidden="1">Sheet1!$B$10</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_lin" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
@@ -26,7 +130,7 @@
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">2</definedName>
   </definedNames>
-  <calcPr calcId="191029" calcCompleted="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -944,12 +1048,12 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-GB" sz="1800" b="0" i="0" baseline="0">
+              <a:rPr lang="en-GB" sz="1000" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
               <a:t>Annual percentage growth in the Australian</a:t>
             </a:r>
-            <a:endParaRPr lang="en-AU">
+            <a:endParaRPr lang="en-AU" sz="1000">
               <a:effectLst/>
             </a:endParaRPr>
           </a:p>
@@ -968,17 +1072,25 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-GB" sz="1800" b="0" i="0" baseline="0">
+              <a:rPr lang="en-GB" sz="1000" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
               <a:t>Wage Price Index between March 2021 - March 2022</a:t>
             </a:r>
-            <a:endParaRPr lang="en-AU">
+            <a:endParaRPr lang="en-AU" sz="1000">
               <a:effectLst/>
             </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.14173985803381098"/>
+          <c:y val="5.2280926964162519E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1015,10 +1127,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.56618392680734264"/>
-          <c:y val="0.4726154274880745"/>
-          <c:w val="0.39705233540066137"/>
-          <c:h val="0.42577327303247053"/>
+          <c:x val="0.4171241779391241"/>
+          <c:y val="0.21201230101648913"/>
+          <c:w val="0.54611202831264316"/>
+          <c:h val="0.68637640535898603"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -1078,7 +1190,7 @@
                   <c:v>2.4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.9</c:v>
+                  <c:v>1.9470000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2.1</c:v>
@@ -1145,7 +1257,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1162,7 +1274,7 @@
         </c:txPr>
         <c:crossAx val="980666368"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
+        <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
@@ -3711,16 +3823,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>498697</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>555628</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>70068</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>266943</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>160247</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>323874</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>28867</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3747,16 +3859,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>140948</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>189888</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>536721</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>155725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>590064</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>102659</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>334876</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>37910</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4417,8 +4529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67D63F77-D626-664F-97E8-D742B7AF639D}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="290" zoomScaleNormal="290" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="201" zoomScaleNormal="290" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4442,7 +4554,7 @@
         <v>27</v>
       </c>
       <c r="B2" s="2">
-        <v>1.9</v>
+        <v>1.9470000000000001</v>
       </c>
       <c r="C2" s="2">
         <v>0</v>

</xml_diff>